<commit_message>
Modifiy word designation in schedule
</commit_message>
<xml_diff>
--- a/Development schedule.xlsx
+++ b/Development schedule.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\동아리개인\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\Web-Graphicer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -50,10 +50,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>프로세스 설계</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>레이아웃 설계</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,7 +78,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>프로세스 구상</t>
+    <t>기능 구상</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>기능 구상/기술 결정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -129,14 +129,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -327,7 +324,7 @@
                     <c:v>레이아웃 설계</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>프로세스 구상</c:v>
+                    <c:v>기능 구상/기술 결정</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>디자인</c:v>
@@ -344,7 +341,7 @@
                     <c:v>화면설계</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>프로세스 설계</c:v>
+                    <c:v>기능 구상</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>프론트엔드</c:v>
@@ -378,7 +375,7 @@
                   <c:v>43021</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43041</c:v>
+                  <c:v>43049</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -484,7 +481,7 @@
                     <c:v>레이아웃 설계</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>프로세스 구상</c:v>
+                    <c:v>기능 구상/기술 결정</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>디자인</c:v>
@@ -501,7 +498,7 @@
                     <c:v>화면설계</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>프로세스 설계</c:v>
+                    <c:v>기능 구상</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>프론트엔드</c:v>
@@ -532,10 +529,10 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -640,7 +637,7 @@
                     <c:v>레이아웃 설계</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>프로세스 구상</c:v>
+                    <c:v>기능 구상/기술 결정</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>디자인</c:v>
@@ -657,7 +654,7 @@
                     <c:v>화면설계</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>프로세스 설계</c:v>
+                    <c:v>기능 구상</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v>프론트엔드</c:v>
@@ -688,7 +685,7 @@
                   <c:v>43021</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>43041</c:v>
+                  <c:v>43049</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>43069</c:v>
@@ -1714,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1747,7 +1744,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="1">
         <v>43001</v>
@@ -1762,7 +1759,7 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" s="1">
         <f>F2</f>
@@ -1778,7 +1775,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -1797,10 +1794,10 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
       <c r="D5" s="1">
         <v>43015</v>
@@ -1815,34 +1812,34 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" s="1">
         <v>43021</v>
       </c>
       <c r="E6">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F6" s="1">
         <f>D6+E6-1</f>
-        <v>43041</v>
+        <v>43049</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" t="s">
         <v>10</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
       </c>
       <c r="D7" s="1">
         <f>F6</f>
-        <v>43041</v>
+        <v>43049</v>
       </c>
       <c r="E7">
-        <v>29</v>
-      </c>
-      <c r="F7" s="2">
+        <v>21</v>
+      </c>
+      <c r="F7" s="1">
         <f>D7+E7-1</f>
         <v>43069</v>
       </c>

</xml_diff>